<commit_message>
Update CMS FOR LED 的调整（LEIVS杭州杭州大厦店）20191120.xlsx
</commit_message>
<xml_diff>
--- a/2019/杭州杭州大厦店/05 系统集成/LED信息/CMS FOR LED 的调整（LEIVS杭州杭州大厦店）20191120.xlsx
+++ b/2019/杭州杭州大厦店/05 系统集成/LED信息/CMS FOR LED 的调整（LEIVS杭州杭州大厦店）20191120.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File Server\Tree Sapling\03 Levi's\gitCube-levisProject\2019\杭州杭州大厦店\05 系统集成\LED信息\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E4DFCF-588C-439D-A609-59BCF5BB333B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE54CFD1-B459-4B00-AC13-2B22D6983019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="14616" tabRatio="805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="14616" tabRatio="805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="屏幕分割" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>A1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -206,6 +206,10 @@
     <t>1920*166</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>杭大</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -215,7 +219,7 @@
     <numFmt numFmtId="176" formatCode="?.#&quot;个&quot;"/>
     <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -306,6 +310,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -529,7 +540,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1">
       <alignment vertical="center"/>
@@ -592,6 +603,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -619,15 +657,6 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -637,23 +666,8 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -748,15 +762,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2369820</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>102153</xdr:rowOff>
+      <xdr:colOff>2346960</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>132633</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -771,7 +785,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2857500" y="1043940"/>
+          <a:off x="2834640" y="1706880"/>
           <a:ext cx="2095500" cy="254553"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -840,6 +854,121 @@
               <a:sym typeface="Helvetica"/>
             </a:rPr>
             <a:t>STB1(1920*166)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1356360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>64053</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C5D555D-BA22-4C96-993E-61C88B95BCF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1226820" y="1112520"/>
+          <a:ext cx="5638800" cy="254553"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="none"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Helvetica"/>
+            </a:rPr>
+            <a:t>STB1(3712*320)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
@@ -2060,7 +2189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0840242B-9A89-4F4D-93E8-1F02C65A3D0D}">
   <dimension ref="A1:IP8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -2089,36 +2218,36 @@
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:250" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="28"/>
+      <c r="L2" s="37"/>
       <c r="IP2" s="10"/>
     </row>
     <row r="3" spans="1:250" ht="27.6" x14ac:dyDescent="0.25">
@@ -2134,14 +2263,14 @@
       <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
       <c r="IP3" s="10"/>
     </row>
     <row r="4" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
@@ -2154,29 +2283,29 @@
       <c r="C4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="32">
         <v>1</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="32">
         <v>1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="32">
         <v>1</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="32">
         <v>1</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="46" t="s">
+      <c r="J4" s="26"/>
+      <c r="K4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="30"/>
+      <c r="L4" s="39"/>
       <c r="IP4" s="10"/>
     </row>
     <row r="5" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
@@ -2189,15 +2318,15 @@
       <c r="C5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="30"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="39"/>
       <c r="IP5" s="10"/>
     </row>
     <row r="6" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
@@ -2210,15 +2339,15 @@
       <c r="C6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="30"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="39"/>
       <c r="IP6" s="10"/>
     </row>
     <row r="7" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
@@ -2251,7 +2380,7 @@
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="23"/>
-      <c r="L7" s="30"/>
+      <c r="L7" s="39"/>
       <c r="IP7" s="10"/>
     </row>
     <row r="8" spans="1:250" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -2283,12 +2412,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -2301,6 +2424,12 @@
     <mergeCell ref="G4:G6"/>
     <mergeCell ref="H4:H6"/>
     <mergeCell ref="D4:D6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2313,10 +2442,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E3"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2330,6 +2459,11 @@
     <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5" ht="22.2" x14ac:dyDescent="0.25">
+      <c r="B1" s="49" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="2" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2">
         <v>896</v>
@@ -2355,10 +2489,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>